<commit_message>
fix: Jenkins test profile execution fixed
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="25">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -131,7 +131,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C440"/>
+  <dimension ref="A1:C449"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -4967,6 +4967,105 @@
         <v>2</v>
       </c>
     </row>
+    <row r="441">
+      <c r="A441" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B441" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C441" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B442" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C442" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B443" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C443" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B444" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C444" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B445" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C445" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B446" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C446" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B447" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C447" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B448" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C448" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B449" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C449" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Replace JavaFaker with DataFaker and update dependencies
- Replaced deprecated JavaFaker with actively maintained DataFaker
- Updated commons-io to resolve compatibility with Apache POI
- Ran code reformatting and optimized imports
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="25">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -131,7 +131,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C449"/>
+  <dimension ref="A1:C451"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -5066,6 +5066,28 @@
         <v>2</v>
       </c>
     </row>
+    <row r="450">
+      <c r="A450" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B450" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C450" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B451" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C451" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Code formatting, import optimization, and locator updates
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="28">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -88,6 +88,15 @@
   <si>
     <t>Countries testing with JDBC</t>
   </si>
+  <si>
+    <t>Fees create and delete functionality</t>
+  </si>
+  <si>
+    <t>Create a Country</t>
+  </si>
+  <si>
+    <t>Create a CitizenShip</t>
+  </si>
 </sst>
 </file>
 
@@ -131,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C451"/>
+  <dimension ref="A1:C504"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -5088,6 +5097,587 @@
         <v>2</v>
       </c>
     </row>
+    <row r="452">
+      <c r="A452" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B452" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C452" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B453" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C453" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B454" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C454" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B455" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C455" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B456" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C456" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B457" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C457" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B458" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C458" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B459" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C459" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B460" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C460" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B461" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C461" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B462" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C462" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B463" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C463" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B464" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C464" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B465" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C465" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B466" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C466" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B467" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C467" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B468" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C468" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B469" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C469" s="0"/>
+    </row>
+    <row r="470">
+      <c r="A470" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B470" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C470" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B471" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C471" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B472" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C472" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B473" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C473" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B474" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C474" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B475" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C475" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B476" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C476" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B477" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C477" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B478" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C478" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B479" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C479" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B480" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C480" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B481" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C481" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B482" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C482" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B483" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C483" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B484" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C484" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B485" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C485" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B486" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C486" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B487" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C487" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B488" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C488" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B489" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C489" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B490" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C490" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B491" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C491" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B492" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C492" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B493" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C493" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B494" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C494" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B495" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C495" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B496" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C496" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B497" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C497" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B498" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C498" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B499" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C499" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B500" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C500" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B501" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C501" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B502" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C502" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B503" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C503" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B504" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C504" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve verifyContainsText with FluentWait and exception handling
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="28">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -140,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C504"/>
+  <dimension ref="A1:C515"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -5678,6 +5678,127 @@
         <v>2</v>
       </c>
     </row>
+    <row r="505">
+      <c r="A505" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B505" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C505" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B506" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C506" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B507" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C507" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B508" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C508" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B509" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C509" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B510" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C510" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B511" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C511" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B512" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C512" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B513" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C513" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B514" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C514" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B515" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C515" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored JDBC data fetch and validation logic - Added null checks for DB connection - Improved exception handling and logging - Ensured clean resource closing with try-finally
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="28">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -140,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C515"/>
+  <dimension ref="A1:C518"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -5799,6 +5799,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="516">
+      <c r="A516" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B516" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C516" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B517" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C517" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B518" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C518" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Configure Cucumber runners with tag filters and reporting plugins
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="29">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -143,7 +143,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C550"/>
+  <dimension ref="A1:C565"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -6187,6 +6187,171 @@
         <v>2</v>
       </c>
     </row>
+    <row r="551">
+      <c r="A551" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B551" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C551" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B552" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C552" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B553" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C553" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B554" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C554" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B555" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C555" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B556" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C556" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B557" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C557" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B558" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C558" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B559" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C559" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B560" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C560" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B561" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C561" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B562" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C562" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B563" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C563" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B564" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C564" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B565" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C565" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Update JDBC test scenario
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="30">
   <si>
     <t>Create and Delete CitizenShip From Excel</t>
   </si>
@@ -100,6 +100,9 @@
   <si>
     <t>Create a country with base name and code (but generate unique)</t>
   </si>
+  <si>
+    <t>Nationality testing with JDBC</t>
+  </si>
 </sst>
 </file>
 
@@ -143,7 +146,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C565"/>
+  <dimension ref="A1:C566"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -6352,6 +6355,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="566">
+      <c r="A566" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B566" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C566" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>